<commit_message>
Comparison bar graph for Mongo insertion rate
Signed-off-by: Jason Rudland <knowlecules@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/REST benchmarks.xlsx
+++ b/docs/REST benchmarks.xlsx
@@ -317,6 +317,150 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Single MongoDB insert per REST request</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$4:$L$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Restify</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Journey</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>rapid-rest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$4:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2546.905509805586</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2724.5481790936337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4001.0669511869833</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3806.1405734585132</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-25"/>
+        <c:axId val="113014272"/>
+        <c:axId val="113000448"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="113014272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113000448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="113000448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113014272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
@@ -1829,16 +1973,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2013,16 +2157,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1304925</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2036,6 +2180,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2333,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
rapid-rest supports enforced query string parameters
</commit_message>
<xml_diff>
--- a/docs/REST benchmarks.xlsx
+++ b/docs/REST benchmarks.xlsx
@@ -84,9 +84,6 @@
     <t>300K</t>
   </si>
   <si>
-    <t>30k MongoDB inserts</t>
-  </si>
-  <si>
     <t>Inserts per second</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Single</t>
+  </si>
+  <si>
+    <t>Single MongoDB inserts</t>
   </si>
 </sst>
 </file>
@@ -157,11 +157,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -233,7 +233,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30k MongoDB inserts Total</c:v>
+                  <c:v>Single MongoDB inserts Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -267,11 +267,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101076992"/>
-        <c:axId val="101078528"/>
+        <c:axId val="123548800"/>
+        <c:axId val="123550336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101076992"/>
+        <c:axId val="123548800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -281,7 +281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101078528"/>
+        <c:crossAx val="123550336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -289,7 +289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101078528"/>
+        <c:axId val="123550336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,7 +300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101076992"/>
+        <c:crossAx val="123548800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -413,11 +413,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="113014272"/>
-        <c:axId val="113000448"/>
+        <c:axId val="124697600"/>
+        <c:axId val="124707584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113014272"/>
+        <c:axId val="124697600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +426,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113000448"/>
+        <c:crossAx val="124707584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -434,7 +434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113000448"/>
+        <c:axId val="124707584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -444,7 +444,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113014272"/>
+        <c:crossAx val="124697600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -510,7 +510,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30k MongoDB inserts</c:v>
+                  <c:v>Single MongoDB inserts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -568,11 +568,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="101115392"/>
-        <c:axId val="101116928"/>
+        <c:axId val="123579392"/>
+        <c:axId val="123581184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101115392"/>
+        <c:axId val="123579392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,7 +581,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101116928"/>
+        <c:crossAx val="123581184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -589,7 +589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101116928"/>
+        <c:axId val="123581184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,7 +599,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101115392"/>
+        <c:crossAx val="123579392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -733,11 +733,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="101329920"/>
-        <c:axId val="101344000"/>
+        <c:axId val="124011264"/>
+        <c:axId val="124012800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101329920"/>
+        <c:axId val="124011264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +746,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101344000"/>
+        <c:crossAx val="124012800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -754,7 +754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101344000"/>
+        <c:axId val="124012800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +770,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="101329920"/>
+        <c:crossAx val="124011264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -900,11 +900,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101376384"/>
-        <c:axId val="101377920"/>
+        <c:axId val="124020992"/>
+        <c:axId val="124035072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101376384"/>
+        <c:axId val="124020992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101377920"/>
+        <c:crossAx val="124035072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -921,7 +921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101377920"/>
+        <c:axId val="124035072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -932,7 +932,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101376384"/>
+        <c:crossAx val="124020992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1027,11 +1027,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101469184"/>
-        <c:axId val="101470976"/>
+        <c:axId val="124046720"/>
+        <c:axId val="124462208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101469184"/>
+        <c:axId val="124046720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1041,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101470976"/>
+        <c:crossAx val="124462208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1049,7 +1049,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101470976"/>
+        <c:axId val="124462208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1059,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101469184"/>
+        <c:crossAx val="124046720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1226,11 +1226,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101503744"/>
-        <c:axId val="101505280"/>
+        <c:axId val="124486400"/>
+        <c:axId val="124487936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101503744"/>
+        <c:axId val="124486400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,7 +1240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101505280"/>
+        <c:crossAx val="124487936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1248,7 +1248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101505280"/>
+        <c:axId val="124487936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,7 +1259,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101503744"/>
+        <c:crossAx val="124486400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1300,15 +1300,23 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>B</a:t>
+              <a:rPr lang="en-CA"/>
+              <a:t>30K Batched versus single </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>MongoDB insert using</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>atched mongo insert rate over REST</a:t>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> REST server</a:t>
             </a:r>
+            <a:endParaRPr lang="en-CA"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1323,8 +1331,8 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:idx val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$W$2:$W$3</c:f>
@@ -1379,21 +1387,78 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Single MongoDB inserts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$4:$L$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Restify</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Journey</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>rapid-rest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$4:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2546.905509805586</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2724.5481790936337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4001.0669511869833</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3806.1405734585132</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="75"/>
+        <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="111863680"/>
-        <c:axId val="118441088"/>
+        <c:axId val="39536128"/>
+        <c:axId val="39537664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111863680"/>
+        <c:axId val="39536128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1402,7 +1467,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118441088"/>
+        <c:crossAx val="39537664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1410,29 +1475,23 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118441088"/>
+        <c:axId val="39537664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9525">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="111863680"/>
+        <c:crossAx val="39536128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -1617,11 +1676,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="53745536"/>
-        <c:axId val="66232704"/>
+        <c:axId val="124556800"/>
+        <c:axId val="124558336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53745536"/>
+        <c:axId val="124556800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1689,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66232704"/>
+        <c:crossAx val="124558336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1638,7 +1697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66232704"/>
+        <c:axId val="124558336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,7 +1707,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53745536"/>
+        <c:crossAx val="124556800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1854,11 +1913,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="66516480"/>
-        <c:axId val="66633728"/>
+        <c:axId val="124670720"/>
+        <c:axId val="124672256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66516480"/>
+        <c:axId val="124670720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,7 +1926,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66633728"/>
+        <c:crossAx val="124672256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1875,7 +1934,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66633728"/>
+        <c:axId val="124672256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1885,7 +1944,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66516480"/>
+        <c:crossAx val="124670720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2095,16 +2154,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2187,16 +2246,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2509,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,31 +2606,31 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="5"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" s="5"/>
+      <c r="W2" s="7"/>
       <c r="AA2" t="s">
         <v>10</v>
       </c>
@@ -2584,16 +2643,16 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M3" t="s">
         <v>3</v>
@@ -2602,10 +2661,10 @@
         <v>5</v>
       </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V3" t="s">
         <v>3</v>
@@ -2631,11 +2690,11 @@
         <f>C$1/B4</f>
         <v>4986.7021276595742</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f>(C4-C$4)/C4</f>
         <v>0</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="5"/>
       <c r="F4" t="s">
         <v>0</v>
       </c>
@@ -2655,7 +2714,7 @@
         <f>M4-I4</f>
         <v>4.2809999999999997</v>
       </c>
-      <c r="K4" s="6"/>
+      <c r="K4" s="5"/>
       <c r="L4" t="s">
         <v>0</v>
       </c>
@@ -2666,11 +2725,11 @@
         <f>N$1/M4</f>
         <v>2546.905509805586</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <f>M4-M$6/M$6</f>
         <v>10.779</v>
       </c>
-      <c r="P4" s="6"/>
+      <c r="P4" s="5"/>
       <c r="Q4" t="s">
         <v>0</v>
       </c>
@@ -2678,7 +2737,7 @@
         <f>M4-G4</f>
         <v>8.32</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S4" s="6">
         <f>V4-G5</f>
         <v>4.3330000000000002</v>
       </c>
@@ -2699,7 +2758,7 @@
         <f>M6</f>
         <v>7.4980000000000002</v>
       </c>
-      <c r="AC4" s="6">
+      <c r="AC4" s="5">
         <f>(AB4-AB$4)/AB4</f>
         <v>0</v>
       </c>
@@ -2715,11 +2774,11 @@
         <f>C$1/B5</f>
         <v>4351.610095735422</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <f>(C5-C$4)/C5</f>
         <v>-0.14594414893617019</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="5"/>
       <c r="F5" t="s">
         <v>1</v>
       </c>
@@ -2739,7 +2798,7 @@
         <f>M5-I5</f>
         <v>3.512999999999999</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="5"/>
       <c r="L5" t="s">
         <v>1</v>
       </c>
@@ -2750,11 +2809,11 @@
         <f>N$1/M5</f>
         <v>2724.5481790936337</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <f>M5-M$6/M$6</f>
         <v>10.010999999999999</v>
       </c>
-      <c r="P5" s="6"/>
+      <c r="P5" s="5"/>
       <c r="Q5" t="s">
         <v>1</v>
       </c>
@@ -2762,7 +2821,7 @@
         <f>M5-G5</f>
         <v>7.5519999999999996</v>
       </c>
-      <c r="S5" s="7">
+      <c r="S5" s="6">
         <f>V5-G6</f>
         <v>4.4220000000000006</v>
       </c>
@@ -2776,7 +2835,7 @@
         <f>W$1/V5</f>
         <v>3806.623524933384</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X5" s="5">
         <f>(W5-W$4)/W5</f>
         <v>-1.1421971252566802E-2</v>
       </c>
@@ -2786,7 +2845,7 @@
       <c r="AB5">
         <v>6.4119999999999999</v>
       </c>
-      <c r="AC5" s="6">
+      <c r="AC5" s="5">
         <f>-(AB5-AB$4)/AB5</f>
         <v>0.16936993137866505</v>
       </c>
@@ -2802,11 +2861,11 @@
         <f>C$1/B6</f>
         <v>8673.026886383348</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f>(C6-C$4)/C6</f>
         <v>0.42503324468085113</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="5"/>
       <c r="F6" t="s">
         <v>2</v>
       </c>
@@ -2826,7 +2885,7 @@
         <f>M6-I6</f>
         <v>0</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="5"/>
       <c r="L6" t="s">
         <v>2</v>
       </c>
@@ -2837,11 +2896,11 @@
         <f>N$1/M6</f>
         <v>4001.0669511869833</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <f>M6-M$6/M$6</f>
         <v>6.4980000000000002</v>
       </c>
-      <c r="P6" s="6"/>
+      <c r="P6" s="5"/>
       <c r="Q6" t="s">
         <v>2</v>
       </c>
@@ -2849,7 +2908,7 @@
         <f>M6-G6</f>
         <v>4.0389999999999997</v>
       </c>
-      <c r="S6" s="7">
+      <c r="S6" s="6">
         <f>V6-G7</f>
         <v>1.1359999999999997</v>
       </c>
@@ -2863,7 +2922,7 @@
         <f>W$1/V6</f>
         <v>6528.8356909684444</v>
       </c>
-      <c r="X6" s="6">
+      <c r="X6" s="5">
         <f>(W6-W$4)/W6</f>
         <v>0.41029260780287474</v>
       </c>
@@ -2873,7 +2932,7 @@
       <c r="AB6">
         <v>5.4359999999999999</v>
       </c>
-      <c r="AC6" s="6">
+      <c r="AC6" s="5">
         <f>-(AB6-AB$4)/AB6</f>
         <v>0.37932303164091247</v>
       </c>
@@ -2889,11 +2948,11 @@
         <f>C$1/B7</f>
         <v>8234.9711776008789</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <f>(C7-C$4)/C7</f>
         <v>0.3944481382978724</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="5"/>
       <c r="F7" t="s">
         <v>9</v>
       </c>
@@ -2913,7 +2972,7 @@
         <f>M7-I7</f>
         <v>0.38399999999999945</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="5"/>
       <c r="L7" t="s">
         <v>9</v>
       </c>
@@ -2924,11 +2983,11 @@
         <f>N$1/M7</f>
         <v>3806.1405734585132</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="5">
         <f>M7-M$6/M$6</f>
         <v>6.8819999999999997</v>
       </c>
-      <c r="P7" s="6"/>
+      <c r="P7" s="5"/>
       <c r="Q7" t="s">
         <v>9</v>
       </c>
@@ -2936,7 +2995,7 @@
         <f>M7-G7</f>
         <v>4.423</v>
       </c>
-      <c r="S7" s="7">
+      <c r="S7" s="6">
         <f>V7-$G$7</f>
         <v>1.5239999999999996</v>
       </c>
@@ -2950,7 +3009,7 @@
         <f>W$1/V7</f>
         <v>6020.4695966285371</v>
       </c>
-      <c r="X7" s="6">
+      <c r="X7" s="5">
         <f>(W7-W$4)/W7</f>
         <v>0.36049794661190965</v>
       </c>
@@ -2960,54 +3019,54 @@
       <c r="AB7">
         <v>5.2370000000000001</v>
       </c>
-      <c r="AC7" s="6">
+      <c r="AC7" s="5">
         <f>-(AB7-AB$4)/AB7</f>
         <v>0.43173572656100823</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K8" s="1"/>
-      <c r="L8" s="6"/>
+      <c r="L8" s="5"/>
       <c r="AA8">
         <v>8</v>
       </c>
       <c r="AB8">
         <v>5.2610000000000001</v>
       </c>
-      <c r="AC8" s="6">
+      <c r="AC8" s="5">
         <f>-(AB8-AB$4)/AB8</f>
         <v>0.42520433377684852</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K9" s="1"/>
-      <c r="L9" s="6"/>
+      <c r="L9" s="5"/>
       <c r="AA9">
         <v>10</v>
       </c>
       <c r="AB9">
         <v>5.1790000000000003</v>
       </c>
-      <c r="AC9" s="6">
+      <c r="AC9" s="5">
         <f>-(AB9-AB$4)/AB9</f>
         <v>0.44776983973740103</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>

</xml_diff>